<commit_message>
- Update cuartos output file
</commit_message>
<xml_diff>
--- a/storage/pedidos/outputCuartosFrios.xlsx
+++ b/storage/pedidos/outputCuartosFrios.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="132" windowWidth="18852" windowHeight="8448" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="132" windowWidth="18852" windowHeight="8448"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Partes" sheetId="1" r:id="rId1"/>
+    <sheet name="Pedido" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Evaporadora</t>
   </si>
@@ -62,12 +62,6 @@
   </si>
   <si>
     <t>PedidoID</t>
-  </si>
-  <si>
-    <t>Notas</t>
-  </si>
-  <si>
-    <t>Esta es una nota de prueba</t>
   </si>
 </sst>
 </file>
@@ -452,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -571,28 +565,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>